<commit_message>
Se soluciono el no poder hacer click en los radiosButton de CFM y perdida, el "setClickable" estaba establecido en el arranque del programa
</commit_message>
<xml_diff>
--- a/datos/ValoresTabla/ListaValoresVelocidad.xlsx
+++ b/datos/ValoresTabla/ListaValoresVelocidad.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="N:\Android\Proy_Android_Studio\HVACTOOLS_v2\datos\ValoresTabla\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{38D69427-9E0F-4F62-AEED-1EC1363B8C2C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1DD63BA2-7374-47CC-BD0B-A6A63E650824}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="21840" windowHeight="13140" xr2:uid="{52BF25ED-9E97-4789-B351-4CC772127720}"/>
+    <workbookView xWindow="21480" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{52BF25ED-9E97-4789-B351-4CC772127720}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -522,8 +522,8 @@
   <dimension ref="A2:K1297"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A1254" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F1268" sqref="F1268:F1297"/>
+      <pane ySplit="2" topLeftCell="A1278" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A447" sqref="A447:G1297"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>